<commit_message>
Add New Languages and Tools again
</commit_message>
<xml_diff>
--- a/checklist.xlsx
+++ b/checklist.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12180" activeTab="1"/>
+    <workbookView windowWidth="28800" windowHeight="12180"/>
   </bookViews>
   <sheets>
     <sheet name="Чек-лист (функциональное тестир" sheetId="1" r:id="rId1"/>
@@ -151,7 +151,7 @@
     </r>
   </si>
   <si>
-    <t>V16</t>
+    <t>V5</t>
   </si>
   <si>
     <r>
@@ -185,7 +185,7 @@
     <t>скринкаст</t>
   </si>
   <si>
-    <t>V17</t>
+    <t>V6</t>
   </si>
   <si>
     <r>
@@ -213,7 +213,7 @@
     <t>MAREV-48</t>
   </si>
   <si>
-    <t>V5</t>
+    <t>V7</t>
   </si>
   <si>
     <r>
@@ -241,7 +241,7 @@
     <t>MAREV-39</t>
   </si>
   <si>
-    <t>V6</t>
+    <t>V8</t>
   </si>
   <si>
     <r>
@@ -269,7 +269,7 @@
     <t>MAREV-40</t>
   </si>
   <si>
-    <t>V7</t>
+    <t>V9</t>
   </si>
   <si>
     <r>
@@ -294,7 +294,7 @@
     </r>
   </si>
   <si>
-    <t>V18</t>
+    <t>V10</t>
   </si>
   <si>
     <r>
@@ -319,7 +319,7 @@
     </r>
   </si>
   <si>
-    <t>V8</t>
+    <t>V11</t>
   </si>
   <si>
     <r>
@@ -347,7 +347,7 @@
     <t>Область ввода станции метро</t>
   </si>
   <si>
-    <t>V9</t>
+    <t>V12</t>
   </si>
   <si>
     <r>
@@ -372,7 +372,7 @@
     </r>
   </si>
   <si>
-    <t>V10</t>
+    <t>V13</t>
   </si>
   <si>
     <r>
@@ -397,7 +397,7 @@
     </r>
   </si>
   <si>
-    <t>V19</t>
+    <t>V14</t>
   </si>
   <si>
     <r>
@@ -422,7 +422,7 @@
     </r>
   </si>
   <si>
-    <t>V11</t>
+    <t>V15</t>
   </si>
   <si>
     <r>
@@ -450,7 +450,7 @@
     <t>MAREV-41</t>
   </si>
   <si>
-    <t>V20</t>
+    <t>V16</t>
   </si>
   <si>
     <r>
@@ -475,7 +475,7 @@
     </r>
   </si>
   <si>
-    <t>V12</t>
+    <t>V17</t>
   </si>
   <si>
     <r>
@@ -500,7 +500,7 @@
     </r>
   </si>
   <si>
-    <t>V13</t>
+    <t>V18</t>
   </si>
   <si>
     <r>
@@ -528,7 +528,7 @@
     <t>MAREV-42</t>
   </si>
   <si>
-    <t>V14</t>
+    <t>V19</t>
   </si>
   <si>
     <r>
@@ -553,7 +553,7 @@
     </r>
   </si>
   <si>
-    <t>V21</t>
+    <t>V20</t>
   </si>
   <si>
     <r>
@@ -578,7 +578,7 @@
     </r>
   </si>
   <si>
-    <t>V22</t>
+    <t>V21</t>
   </si>
   <si>
     <r>
@@ -603,7 +603,7 @@
     </r>
   </si>
   <si>
-    <t>V23</t>
+    <t>V22</t>
   </si>
   <si>
     <r>
@@ -631,7 +631,7 @@
     <t>Карточка маршрута</t>
   </si>
   <si>
-    <t>V24</t>
+    <t>V23</t>
   </si>
   <si>
     <r>
@@ -656,7 +656,7 @@
     </r>
   </si>
   <si>
-    <t>V25</t>
+    <t>V24</t>
   </si>
   <si>
     <r>
@@ -681,7 +681,7 @@
     </r>
   </si>
   <si>
-    <t>V26</t>
+    <t>V25</t>
   </si>
   <si>
     <r>
@@ -709,7 +709,7 @@
     <t>MAREV-53</t>
   </si>
   <si>
-    <t>V27</t>
+    <t>V26</t>
   </si>
   <si>
     <r>
@@ -737,7 +737,7 @@
     <t>MAREV-54</t>
   </si>
   <si>
-    <t>V28</t>
+    <t>V27</t>
   </si>
   <si>
     <r>
@@ -765,7 +765,7 @@
     <t>MAREV-50</t>
   </si>
   <si>
-    <t>V29</t>
+    <t>V28</t>
   </si>
   <si>
     <r>
@@ -796,7 +796,7 @@
     <t>Карточка станции</t>
   </si>
   <si>
-    <t>V30</t>
+    <t>V29</t>
   </si>
   <si>
     <r>
@@ -821,7 +821,7 @@
     </r>
   </si>
   <si>
-    <t>V31</t>
+    <t>V30</t>
   </si>
   <si>
     <r>
@@ -846,7 +846,7 @@
     </r>
   </si>
   <si>
-    <t>V32</t>
+    <t>V31</t>
   </si>
   <si>
     <r>
@@ -871,7 +871,7 @@
     </r>
   </si>
   <si>
-    <t>V33</t>
+    <t>V32</t>
   </si>
   <si>
     <r>
@@ -899,7 +899,7 @@
     <t>Работа при отсутствии интернета</t>
   </si>
   <si>
-    <t>V15</t>
+    <t>V33</t>
   </si>
   <si>
     <r>
@@ -934,58 +934,58 @@
     <t>Основные проверки</t>
   </si>
   <si>
-    <t>D66</t>
+    <t>D1</t>
   </si>
   <si>
     <t>При установке новой версии приложения запрашивается местоположение.</t>
   </si>
   <si>
-    <t>D67</t>
+    <t>D2</t>
   </si>
   <si>
     <t>После обновления приложения сохраняются настройки, установленные в старой версии приложения.</t>
   </si>
   <si>
-    <t>D68</t>
+    <t>D3</t>
   </si>
   <si>
     <t>После обновления приложения сохраняются разрешения, выданные в старой версии приложения.</t>
   </si>
   <si>
-    <t>D69</t>
+    <t>D4</t>
   </si>
   <si>
     <t>После полной остановки приложения при новом запуске сохраняются настройки, история и разрешения.</t>
   </si>
   <si>
-    <t>D70</t>
+    <t>D5</t>
   </si>
   <si>
     <t>После полной остановки приложения при новом запуске не сохраняются введённые станции и построенные маршруты.</t>
   </si>
   <si>
-    <t>D1</t>
+    <t>D6</t>
   </si>
   <si>
     <t>При тапе по иконке приложения появляется экран-заставка Яндекс Метро. Затем показывается карта метро и поле ввода.</t>
   </si>
   <si>
-    <t>D2</t>
+    <t>D7</t>
   </si>
   <si>
     <t>При первом запуске запуске приложения после стартового баннера появляется попап с запросом доступа к данным местоположения устройства. Есть возможность "Разрешить" и "Отклонить"</t>
   </si>
   <si>
-    <t>D3</t>
+    <t>D8</t>
   </si>
   <si>
     <t>При сворачивании-разворачивании приложения информация о станциях и маршруте сохраняется и отображается на экране.</t>
   </si>
   <si>
-    <t>D4</t>
-  </si>
-  <si>
-    <t>D5</t>
+    <t>D9</t>
+  </si>
+  <si>
+    <t>D10</t>
   </si>
   <si>
     <r>
@@ -1010,7 +1010,7 @@
     </r>
   </si>
   <si>
-    <t>D6</t>
+    <t>D11</t>
   </si>
   <si>
     <r>
@@ -1035,7 +1035,7 @@
     </r>
   </si>
   <si>
-    <t>D7</t>
+    <t>D12</t>
   </si>
   <si>
     <r>
@@ -1060,7 +1060,7 @@
     </r>
   </si>
   <si>
-    <t>D8</t>
+    <t>D13</t>
   </si>
   <si>
     <r>
@@ -1085,7 +1085,7 @@
     </r>
   </si>
   <si>
-    <t>D9</t>
+    <t>D14</t>
   </si>
   <si>
     <r>
@@ -1110,7 +1110,7 @@
     </r>
   </si>
   <si>
-    <t>D10</t>
+    <t>D15</t>
   </si>
   <si>
     <r>
@@ -1135,7 +1135,7 @@
     </r>
   </si>
   <si>
-    <t>D11</t>
+    <t>D16</t>
   </si>
   <si>
     <r>
@@ -1160,7 +1160,7 @@
     </r>
   </si>
   <si>
-    <t>D12</t>
+    <t>D17</t>
   </si>
   <si>
     <r>
@@ -1185,13 +1185,13 @@
     </r>
   </si>
   <si>
-    <t>D13</t>
+    <t>D18</t>
   </si>
   <si>
     <t>Приложение открывается и выполняет свои функции с сотовой связью.</t>
   </si>
   <si>
-    <t>D14</t>
+    <t>D19</t>
   </si>
   <si>
     <t>Приложение открывается и работает с Wi-Fi</t>
@@ -1200,7 +1200,7 @@
     <t>Карта метро</t>
   </si>
   <si>
-    <t>D15</t>
+    <t>D20</t>
   </si>
   <si>
     <r>
@@ -1225,7 +1225,7 @@
     </r>
   </si>
   <si>
-    <t>D16</t>
+    <t>D21</t>
   </si>
   <si>
     <r>
@@ -1250,7 +1250,7 @@
     </r>
   </si>
   <si>
-    <t>D17</t>
+    <t>D22</t>
   </si>
   <si>
     <r>
@@ -1275,7 +1275,7 @@
     </r>
   </si>
   <si>
-    <t>D18</t>
+    <t>D23</t>
   </si>
   <si>
     <r>
@@ -1300,7 +1300,7 @@
     </r>
   </si>
   <si>
-    <t>D19</t>
+    <t>D24</t>
   </si>
   <si>
     <r>
@@ -1325,7 +1325,7 @@
     </r>
   </si>
   <si>
-    <t>D20</t>
+    <t>D25</t>
   </si>
   <si>
     <r>
@@ -1350,7 +1350,7 @@
     </r>
   </si>
   <si>
-    <t>D21</t>
+    <t>D26</t>
   </si>
   <si>
     <r>
@@ -1375,7 +1375,7 @@
     </r>
   </si>
   <si>
-    <t>D26</t>
+    <t>D27</t>
   </si>
   <si>
     <r>
@@ -1400,7 +1400,7 @@
     </r>
   </si>
   <si>
-    <t>D29</t>
+    <t>D28</t>
   </si>
   <si>
     <r>
@@ -1425,7 +1425,7 @@
     </r>
   </si>
   <si>
-    <t>D30</t>
+    <t>D29</t>
   </si>
   <si>
     <r>
@@ -1450,7 +1450,7 @@
     </r>
   </si>
   <si>
-    <t>D31</t>
+    <t>D30</t>
   </si>
   <si>
     <r>
@@ -1475,25 +1475,25 @@
     </r>
   </si>
   <si>
+    <t>D31</t>
+  </si>
+  <si>
+    <t>В портретной ориентации окно разворачивается свайпом вверх. Откроется детальная информация о маршруте.</t>
+  </si>
+  <si>
+    <t>D32</t>
+  </si>
+  <si>
+    <t>При повороте устройства горизонтально в альбомной ориентации окно с областью ввода отображается в левом нижнем углу экрана</t>
+  </si>
+  <si>
     <t>D33</t>
   </si>
   <si>
-    <t>В портретной ориентации окно разворачивается свайпом вверх. Откроется детальная информация о маршруте.</t>
-  </si>
-  <si>
-    <t>D35</t>
-  </si>
-  <si>
-    <t>При повороте устройства горизонтально в альбомной ориентации окно с областью ввода отображается в левом нижнем углу экрана</t>
-  </si>
-  <si>
-    <t>D36</t>
-  </si>
-  <si>
     <t>При повороте устройства вверх ногами ориентация остаётся альбомной, окно с областью ввода отображается в левом нижнем углу.</t>
   </si>
   <si>
-    <t>D46</t>
+    <t>D34</t>
   </si>
   <si>
     <r>
@@ -1521,7 +1521,7 @@
     <t>Настройки</t>
   </si>
   <si>
-    <t>D52</t>
+    <t>D35</t>
   </si>
   <si>
     <r>
@@ -1546,7 +1546,7 @@
     </r>
   </si>
   <si>
-    <t>D53</t>
+    <t>D36</t>
   </si>
   <si>
     <r>
@@ -1571,7 +1571,7 @@
     </r>
   </si>
   <si>
-    <t>D54</t>
+    <t>D37</t>
   </si>
   <si>
     <r>
@@ -1596,7 +1596,7 @@
     </r>
   </si>
   <si>
-    <t>D61</t>
+    <t>D38</t>
   </si>
   <si>
     <r>
@@ -1621,7 +1621,7 @@
     </r>
   </si>
   <si>
-    <t>D63</t>
+    <t>D39</t>
   </si>
   <si>
     <r>
@@ -1646,7 +1646,7 @@
     </r>
   </si>
   <si>
-    <t>D64</t>
+    <t>D40</t>
   </si>
   <si>
     <r>
@@ -1671,7 +1671,7 @@
     </r>
   </si>
   <si>
-    <t>D65</t>
+    <t>D41</t>
   </si>
   <si>
     <r>
@@ -2483,7 +2483,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2556,16 +2556,13 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="49">
@@ -3044,18 +3041,18 @@
   </sheetPr>
   <dimension ref="A1:I1038"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomLeft" activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6285714285714" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="3.87619047619048" customWidth="1"/>
+    <col min="1" max="1" width="5" customWidth="1"/>
     <col min="2" max="2" width="97.2476190476191" customWidth="1"/>
-    <col min="3" max="3" width="7.75238095238095" customWidth="1"/>
-    <col min="4" max="4" width="10.752380952381" customWidth="1"/>
+    <col min="3" max="3" width="9.14285714285714" customWidth="1"/>
+    <col min="4" max="4" width="22.1428571428571" customWidth="1"/>
     <col min="5" max="5" width="11" customWidth="1"/>
     <col min="6" max="6" width="12.6285714285714" customWidth="1"/>
   </cols>
@@ -3068,7 +3065,7 @@
       <c r="F1" s="23"/>
       <c r="G1" s="23"/>
       <c r="H1" s="23"/>
-      <c r="I1" s="32"/>
+      <c r="I1" s="31"/>
     </row>
     <row r="2" ht="38.25" spans="1:4">
       <c r="A2" s="2" t="s">
@@ -3092,7 +3089,7 @@
       <c r="C3" s="5"/>
       <c r="D3" s="6"/>
     </row>
-    <row r="4" ht="23.25" customHeight="1" spans="1:4">
+    <row r="4" ht="24" customHeight="1" spans="1:4">
       <c r="A4" s="7" t="s">
         <v>6</v>
       </c>
@@ -3104,7 +3101,7 @@
       </c>
       <c r="D4" s="26"/>
     </row>
-    <row r="5" ht="27.75" customHeight="1" spans="1:4">
+    <row r="5" ht="45" customHeight="1" spans="1:4">
       <c r="A5" s="7" t="s">
         <v>9</v>
       </c>
@@ -3140,7 +3137,7 @@
       </c>
       <c r="D7" s="26"/>
     </row>
-    <row r="8" ht="18" customHeight="1" spans="1:5">
+    <row r="8" ht="18" customHeight="1" spans="1:4">
       <c r="A8" s="17" t="s">
         <v>15</v>
       </c>
@@ -3153,18 +3150,16 @@
       <c r="D8" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="28"/>
-    </row>
-    <row r="9" ht="16.5" customHeight="1" spans="1:5">
+    </row>
+    <row r="9" ht="16.5" customHeight="1" spans="1:4">
       <c r="A9" s="21"/>
       <c r="B9" s="21"/>
       <c r="C9" s="21"/>
       <c r="D9" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="E9" s="28"/>
-    </row>
-    <row r="10" ht="19.5" customHeight="1" spans="1:5">
+    </row>
+    <row r="10" ht="19.5" customHeight="1" spans="1:4">
       <c r="A10" s="17" t="s">
         <v>20</v>
       </c>
@@ -3177,18 +3172,16 @@
       <c r="D10" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="E10" s="28"/>
-    </row>
-    <row r="11" ht="18" customHeight="1" spans="1:5">
+    </row>
+    <row r="11" ht="18" customHeight="1" spans="1:4">
       <c r="A11" s="21"/>
       <c r="B11" s="21"/>
       <c r="C11" s="21"/>
       <c r="D11" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="E11" s="28"/>
-    </row>
-    <row r="12" ht="21.75" customHeight="1" spans="1:5">
+    </row>
+    <row r="12" ht="21.75" customHeight="1" spans="1:4">
       <c r="A12" s="17" t="s">
         <v>23</v>
       </c>
@@ -3201,18 +3194,16 @@
       <c r="D12" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="E12" s="28"/>
-    </row>
-    <row r="13" ht="18.75" customHeight="1" spans="1:5">
+    </row>
+    <row r="13" ht="18.75" customHeight="1" spans="1:4">
       <c r="A13" s="21"/>
       <c r="B13" s="21"/>
       <c r="C13" s="21"/>
       <c r="D13" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="E13" s="29"/>
-    </row>
-    <row r="14" ht="17.25" customHeight="1" spans="1:5">
+    </row>
+    <row r="14" ht="17.25" customHeight="1" spans="1:4">
       <c r="A14" s="17" t="s">
         <v>26</v>
       </c>
@@ -3225,18 +3216,16 @@
       <c r="D14" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="E14" s="29"/>
-    </row>
-    <row r="15" ht="19.5" customHeight="1" spans="1:5">
+    </row>
+    <row r="15" ht="19.5" customHeight="1" spans="1:4">
       <c r="A15" s="21"/>
       <c r="B15" s="21"/>
       <c r="C15" s="21"/>
       <c r="D15" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="E15" s="29"/>
-    </row>
-    <row r="16" ht="25.5" customHeight="1" spans="1:5">
+    </row>
+    <row r="16" ht="39" customHeight="1" spans="1:4">
       <c r="A16" s="7" t="s">
         <v>29</v>
       </c>
@@ -3247,9 +3236,8 @@
         <v>8</v>
       </c>
       <c r="D16" s="26"/>
-      <c r="E16" s="29"/>
-    </row>
-    <row r="17" ht="27" customHeight="1" spans="1:5">
+    </row>
+    <row r="17" ht="39" customHeight="1" spans="1:4">
       <c r="A17" s="7" t="s">
         <v>31</v>
       </c>
@@ -3260,7 +3248,6 @@
         <v>8</v>
       </c>
       <c r="D17" s="26"/>
-      <c r="E17" s="29"/>
     </row>
     <row r="18" ht="38.25" customHeight="1" spans="1:4">
       <c r="A18" s="7" t="s">
@@ -3294,7 +3281,7 @@
       </c>
       <c r="D20" s="26"/>
     </row>
-    <row r="21" ht="39" customHeight="1" spans="1:5">
+    <row r="21" ht="39" customHeight="1" spans="1:4">
       <c r="A21" s="7" t="s">
         <v>38</v>
       </c>
@@ -3305,9 +3292,8 @@
         <v>8</v>
       </c>
       <c r="D21" s="26"/>
-      <c r="E21" s="29"/>
-    </row>
-    <row r="22" ht="26.25" customHeight="1" spans="1:5">
+    </row>
+    <row r="22" ht="26.25" customHeight="1" spans="1:4">
       <c r="A22" s="7" t="s">
         <v>40</v>
       </c>
@@ -3317,10 +3303,9 @@
       <c r="C22" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D22" s="30"/>
-      <c r="E22" s="29"/>
-    </row>
-    <row r="23" ht="16.5" customHeight="1" spans="1:5">
+      <c r="D22" s="28"/>
+    </row>
+    <row r="23" ht="16.5" customHeight="1" spans="1:4">
       <c r="A23" s="17" t="s">
         <v>42</v>
       </c>
@@ -3333,18 +3318,16 @@
       <c r="D23" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="E23" s="29"/>
-    </row>
-    <row r="24" ht="12.75" customHeight="1" spans="1:5">
+    </row>
+    <row r="24" ht="12.75" customHeight="1" spans="1:4">
       <c r="A24" s="21"/>
       <c r="B24" s="21"/>
       <c r="C24" s="21"/>
       <c r="D24" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="E24" s="29"/>
-    </row>
-    <row r="25" ht="18.75" customHeight="1" spans="1:5">
+    </row>
+    <row r="25" ht="18.75" customHeight="1" spans="1:4">
       <c r="A25" s="17" t="s">
         <v>45</v>
       </c>
@@ -3357,18 +3340,16 @@
       <c r="D25" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="E25" s="29"/>
-    </row>
-    <row r="26" ht="18" customHeight="1" spans="1:5">
+    </row>
+    <row r="26" ht="18" customHeight="1" spans="1:4">
       <c r="A26" s="21"/>
       <c r="B26" s="21"/>
       <c r="C26" s="21"/>
       <c r="D26" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="E26" s="29"/>
-    </row>
-    <row r="27" ht="29.25" customHeight="1" spans="1:5">
+    </row>
+    <row r="27" ht="29.25" customHeight="1" spans="1:4">
       <c r="A27" s="7" t="s">
         <v>47</v>
       </c>
@@ -3378,10 +3359,9 @@
       <c r="C27" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D27" s="31"/>
-      <c r="E27" s="29"/>
-    </row>
-    <row r="28" ht="27" customHeight="1" spans="1:5">
+      <c r="D27" s="29"/>
+    </row>
+    <row r="28" ht="27" customHeight="1" spans="1:4">
       <c r="A28" s="17" t="s">
         <v>49</v>
       </c>
@@ -3394,18 +3374,16 @@
       <c r="D28" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="E28" s="29"/>
-    </row>
-    <row r="29" ht="24.75" customHeight="1" spans="1:5">
+    </row>
+    <row r="29" ht="24.75" customHeight="1" spans="1:4">
       <c r="A29" s="21"/>
       <c r="B29" s="21"/>
       <c r="C29" s="21"/>
       <c r="D29" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="E29" s="29"/>
-    </row>
-    <row r="30" ht="27.75" customHeight="1" spans="1:5">
+    </row>
+    <row r="30" ht="27.75" customHeight="1" spans="1:4">
       <c r="A30" s="7" t="s">
         <v>52</v>
       </c>
@@ -3416,9 +3394,8 @@
         <v>8</v>
       </c>
       <c r="D30" s="26"/>
-      <c r="E30" s="29"/>
-    </row>
-    <row r="31" ht="26.25" customHeight="1" spans="1:5">
+    </row>
+    <row r="31" ht="26.25" customHeight="1" spans="1:4">
       <c r="A31" s="17" t="s">
         <v>54</v>
       </c>
@@ -3429,9 +3406,8 @@
         <v>8</v>
       </c>
       <c r="D31" s="26"/>
-      <c r="E31" s="29"/>
-    </row>
-    <row r="32" ht="26.25" customHeight="1" spans="1:5">
+    </row>
+    <row r="32" ht="26.25" customHeight="1" spans="1:4">
       <c r="A32" s="7" t="s">
         <v>56</v>
       </c>
@@ -3442,9 +3418,8 @@
         <v>8</v>
       </c>
       <c r="D32" s="26"/>
-      <c r="E32" s="29"/>
-    </row>
-    <row r="33" ht="26.25" customHeight="1" spans="1:5">
+    </row>
+    <row r="33" ht="26.25" customHeight="1" spans="1:4">
       <c r="A33" s="7" t="s">
         <v>58</v>
       </c>
@@ -3455,7 +3430,6 @@
         <v>8</v>
       </c>
       <c r="D33" s="26"/>
-      <c r="E33" s="29"/>
     </row>
     <row r="34" ht="17.25" customHeight="1" spans="1:4">
       <c r="A34" s="24" t="s">
@@ -3465,7 +3439,7 @@
       <c r="C34" s="5"/>
       <c r="D34" s="6"/>
     </row>
-    <row r="35" ht="27" customHeight="1" spans="1:5">
+    <row r="35" ht="39" customHeight="1" spans="1:4">
       <c r="A35" s="7" t="s">
         <v>61</v>
       </c>
@@ -3476,9 +3450,8 @@
         <v>8</v>
       </c>
       <c r="D35" s="26"/>
-      <c r="E35" s="29"/>
-    </row>
-    <row r="36" ht="35.25" customHeight="1" spans="1:5">
+    </row>
+    <row r="36" ht="41" customHeight="1" spans="1:4">
       <c r="A36" s="7" t="s">
         <v>63</v>
       </c>
@@ -3489,9 +3462,8 @@
         <v>8</v>
       </c>
       <c r="D36" s="26"/>
-      <c r="E36" s="29"/>
-    </row>
-    <row r="37" ht="18.75" customHeight="1" spans="1:5">
+    </row>
+    <row r="37" ht="18.75" customHeight="1" spans="1:4">
       <c r="A37" s="17" t="s">
         <v>65</v>
       </c>
@@ -3504,18 +3476,16 @@
       <c r="D37" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="E37" s="29"/>
-    </row>
-    <row r="38" ht="21" customHeight="1" spans="1:5">
+    </row>
+    <row r="38" ht="21" customHeight="1" spans="1:4">
       <c r="A38" s="21"/>
       <c r="B38" s="21"/>
       <c r="C38" s="21"/>
       <c r="D38" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="E38" s="29"/>
-    </row>
-    <row r="39" ht="20.25" customHeight="1" spans="1:5">
+    </row>
+    <row r="39" ht="20.25" customHeight="1" spans="1:4">
       <c r="A39" s="17" t="s">
         <v>68</v>
       </c>
@@ -3528,18 +3498,16 @@
       <c r="D39" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="E39" s="29"/>
-    </row>
-    <row r="40" ht="14.25" customHeight="1" spans="1:5">
-      <c r="A40" s="21"/>
+    </row>
+    <row r="40" ht="14.25" customHeight="1" spans="1:4">
+      <c r="A40" s="30"/>
       <c r="B40" s="21"/>
       <c r="C40" s="21"/>
       <c r="D40" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="E40" s="29"/>
-    </row>
-    <row r="41" ht="17.25" customHeight="1" spans="1:5">
+    </row>
+    <row r="41" ht="17.25" customHeight="1" spans="1:4">
       <c r="A41" s="17" t="s">
         <v>71</v>
       </c>
@@ -3552,18 +3520,16 @@
       <c r="D41" s="20" t="s">
         <v>73</v>
       </c>
-      <c r="E41" s="29"/>
-    </row>
-    <row r="42" ht="18" customHeight="1" spans="1:5">
-      <c r="A42" s="21"/>
+    </row>
+    <row r="42" ht="18" customHeight="1" spans="1:4">
+      <c r="A42" s="30"/>
       <c r="B42" s="21"/>
       <c r="C42" s="21"/>
       <c r="D42" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="E42" s="29"/>
-    </row>
-    <row r="43" ht="17.25" customHeight="1" spans="1:5">
+    </row>
+    <row r="43" ht="17.25" customHeight="1" spans="1:4">
       <c r="A43" s="17" t="s">
         <v>74</v>
       </c>
@@ -3576,16 +3542,14 @@
       <c r="D43" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="E43" s="29"/>
-    </row>
-    <row r="44" ht="21" customHeight="1" spans="1:5">
-      <c r="A44" s="21"/>
+    </row>
+    <row r="44" ht="21" customHeight="1" spans="1:4">
+      <c r="A44" s="30"/>
       <c r="B44" s="21"/>
       <c r="C44" s="21"/>
       <c r="D44" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="E44" s="29"/>
     </row>
     <row r="45" ht="17.25" customHeight="1" spans="1:4">
       <c r="A45" s="24" t="s">
@@ -3595,7 +3559,7 @@
       <c r="C45" s="5"/>
       <c r="D45" s="6"/>
     </row>
-    <row r="46" ht="25.5" customHeight="1" spans="1:5">
+    <row r="46" ht="25.5" customHeight="1" spans="1:4">
       <c r="A46" s="7" t="s">
         <v>78</v>
       </c>
@@ -3606,9 +3570,8 @@
         <v>8</v>
       </c>
       <c r="D46" s="26"/>
-      <c r="E46" s="29"/>
-    </row>
-    <row r="47" ht="41.25" customHeight="1" spans="1:5">
+    </row>
+    <row r="47" ht="41.25" customHeight="1" spans="1:4">
       <c r="A47" s="7" t="s">
         <v>80</v>
       </c>
@@ -3619,9 +3582,8 @@
         <v>8</v>
       </c>
       <c r="D47" s="26"/>
-      <c r="E47" s="29"/>
-    </row>
-    <row r="48" ht="41.25" customHeight="1" spans="1:5">
+    </row>
+    <row r="48" ht="41.25" customHeight="1" spans="1:4">
       <c r="A48" s="7" t="s">
         <v>82</v>
       </c>
@@ -3632,9 +3594,8 @@
         <v>8</v>
       </c>
       <c r="D48" s="26"/>
-      <c r="E48" s="29"/>
-    </row>
-    <row r="49" ht="39" customHeight="1" spans="1:5">
+    </row>
+    <row r="49" ht="39" customHeight="1" spans="1:4">
       <c r="A49" s="7" t="s">
         <v>84</v>
       </c>
@@ -3645,7 +3606,6 @@
         <v>8</v>
       </c>
       <c r="D49" s="26"/>
-      <c r="E49" s="29"/>
     </row>
     <row r="50" customHeight="1" spans="1:4">
       <c r="A50" s="24" t="s">
@@ -3678,37 +3638,37 @@
       </c>
     </row>
     <row r="53" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A53" s="32"/>
+      <c r="A53" s="31"/>
     </row>
     <row r="54" ht="26.25" customHeight="1" spans="1:1">
-      <c r="A54" s="32"/>
+      <c r="A54" s="31"/>
     </row>
     <row r="55" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A55" s="32"/>
+      <c r="A55" s="31"/>
     </row>
     <row r="56" ht="42" customHeight="1" spans="1:1">
-      <c r="A56" s="32"/>
+      <c r="A56" s="31"/>
     </row>
     <row r="57" ht="15.75" customHeight="1" spans="1:1">
-      <c r="A57" s="32"/>
+      <c r="A57" s="31"/>
     </row>
     <row r="58" ht="17.25" customHeight="1" spans="1:1">
-      <c r="A58" s="32"/>
+      <c r="A58" s="31"/>
     </row>
     <row r="59" ht="27.75" customHeight="1" spans="1:1">
-      <c r="A59" s="32"/>
+      <c r="A59" s="31"/>
     </row>
     <row r="60" ht="27.75" customHeight="1" spans="1:1">
-      <c r="A60" s="32"/>
+      <c r="A60" s="31"/>
     </row>
     <row r="61" ht="27.75" customHeight="1" spans="1:1">
-      <c r="A61" s="32"/>
+      <c r="A61" s="31"/>
     </row>
     <row r="62" ht="27.75" customHeight="1" spans="1:1">
-      <c r="A62" s="32"/>
+      <c r="A62" s="31"/>
     </row>
     <row r="63" ht="27.75" customHeight="1" spans="1:1">
-      <c r="A63" s="32"/>
+      <c r="A63" s="31"/>
     </row>
     <row r="64" ht="15.75" customHeight="1"/>
     <row r="65" ht="15.75" customHeight="1"/>
@@ -4799,10 +4759,10 @@
   </sheetPr>
   <dimension ref="A1:D967"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="E40" sqref="E40"/>
+      <selection pane="bottomLeft" activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6285714285714" defaultRowHeight="15" customHeight="1" outlineLevelCol="3"/>
@@ -4810,7 +4770,7 @@
     <col min="1" max="1" width="4.87619047619048" customWidth="1"/>
     <col min="2" max="2" width="99.5047619047619" customWidth="1"/>
     <col min="3" max="3" width="9.57142857142857" customWidth="1"/>
-    <col min="4" max="4" width="21.7142857142857" customWidth="1"/>
+    <col min="4" max="4" width="21.5714285714286" customWidth="1"/>
     <col min="5" max="5" width="22.247619047619" customWidth="1"/>
     <col min="9" max="9" width="13.5047619047619" customWidth="1"/>
     <col min="10" max="10" width="25.752380952381" customWidth="1"/>

</xml_diff>